<commit_message>
updated CPI files 1949-2024 version 1
</commit_message>
<xml_diff>
--- a/annual_CPI_movement_1949_2018.xlsx
+++ b/annual_CPI_movement_1949_2018.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0252F60-038D-434C-9A8F-11AF76525659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="326">
   <si>
     <t>Figure 1: Annual CPI movement (%)</t>
   </si>
@@ -25,37 +29,7 @@
     <t>Annual CPI Movement (%)</t>
   </si>
   <si>
-    <t>Sep-48</t>
-  </si>
-  <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>Dec-48</t>
-  </si>
-  <si>
-    <t>Mar-49</t>
-  </si>
-  <si>
-    <t>Jun-49</t>
-  </si>
-  <si>
-    <t>Sep-49</t>
-  </si>
-  <si>
-    <t>Dec-49</t>
-  </si>
-  <si>
-    <t>Mar-50</t>
-  </si>
-  <si>
-    <t>Jun-50</t>
-  </si>
-  <si>
-    <t>Sep-50</t>
-  </si>
-  <si>
-    <t>Dec-50</t>
   </si>
   <si>
     <t>Mar-51</t>
@@ -1024,22 +998,27 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -1061,11 +1040,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1404,21 +1386,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C334"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.14" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1429,3333 +1416,3336 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>17777</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>17868</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>17958</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>18050</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>18142</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2">
         <v>10.8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>18233</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2">
         <v>7.9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>18323</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="2">
         <v>7.7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>18415</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="2">
         <v>7.5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>18507</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="2">
         <v>7.3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>18598</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="2">
         <v>12.2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>15</v>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" s="2">
         <v>14.3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>16</v>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="2">
-        <v>18.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="2">
         <v>20.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>18</v>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" s="2">
         <v>23.9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>19</v>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="2">
         <v>22.9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>20</v>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" s="2">
-        <v>19.6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>19.600000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>22</v>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" s="2">
         <v>10.5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>23</v>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" s="2">
         <v>6.8</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>24</v>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="2">
-        <v>4.9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" s="2">
         <v>4.8</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>26</v>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" s="2">
         <v>1.6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>27</v>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" s="2">
         <v>3.2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>28</v>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" s="2">
         <v>1.6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>29</v>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" s="2">
         <v>1.6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>32</v>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>34</v>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" s="2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>35</v>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" s="2">
         <v>3.1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>36</v>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C33" s="2">
         <v>3.1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>37</v>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34" s="2">
         <v>6.1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>38</v>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C35" s="2">
         <v>7.6</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>39</v>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C36" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>40</v>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>41</v>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38" s="2">
         <v>2.9</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>42</v>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C39" s="2">
         <v>1.4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>43</v>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C40" s="2">
         <v>1.4</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>44</v>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41" s="2">
         <v>1.4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>45</v>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>46</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>47</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44" s="2">
         <v>1.4</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>48</v>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45" s="2">
         <v>1.4</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>49</v>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46" s="2">
         <v>1.4</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>50</v>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C47" s="2">
         <v>2.8</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>51</v>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C48" s="2">
         <v>2.7</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>52</v>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C49" s="2">
         <v>2.7</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>53</v>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C50" s="2">
-        <v>4.1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>54</v>
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C51" s="2">
-        <v>4.1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>55</v>
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C52" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>56</v>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C53" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>57</v>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="B54" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C54" s="2">
         <v>3.9</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>58</v>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C55" s="2">
         <v>1.3</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>59</v>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>60</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="B57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>61</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C58" s="2">
         <v>-1.3</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>62</v>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C59" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>63</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C60" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>64</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C61" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>65</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C62" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>66</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C63" s="2">
         <v>1.3</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>67</v>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C64" s="2">
         <v>1.3</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>68</v>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B65" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C65" s="2">
         <v>2.6</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>69</v>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C66" s="2">
         <v>2.6</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>70</v>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="B67" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C67" s="2">
         <v>2.5</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>71</v>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C68" s="2">
         <v>3.8</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>72</v>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B69" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C69" s="2">
         <v>2.5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>73</v>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C70" s="2">
         <v>3.8</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>74</v>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C71" s="2">
         <v>3.7</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>75</v>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="B72" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C72" s="2">
         <v>3.7</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>76</v>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C73" s="2">
-        <v>4.9</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>77</v>
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C74" s="2">
         <v>3.6</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>78</v>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C75" s="2">
         <v>2.4</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>79</v>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C76" s="2">
         <v>2.4</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>80</v>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="B77" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C77" s="2">
-        <v>2.3</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>81</v>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C78" s="2">
         <v>3.5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>82</v>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="B79" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C79" s="2">
         <v>4.7</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>83</v>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C80" s="2">
         <v>3.4</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>84</v>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="B81" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C81" s="2">
         <v>3.4</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>85</v>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C82" s="2">
-        <v>2.2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>86</v>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="B83" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C83" s="2">
-        <v>2.2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>87</v>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="B84" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C84" s="2">
-        <v>2.2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>88</v>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="B85" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C85" s="2">
         <v>3.3</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>89</v>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="B86" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C86" s="2">
         <v>3.3</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>90</v>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="B87" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C87" s="2">
         <v>3.3</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>91</v>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="B88" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C88" s="2">
         <v>3.3</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>92</v>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="B89" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C89" s="2">
         <v>2.1</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>93</v>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="B90" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C90" s="2">
         <v>3.2</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>94</v>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="B91" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C91" s="2">
         <v>3.2</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>95</v>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="B92" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C92" s="2">
         <v>5.3</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>96</v>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="B93" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C93" s="2">
         <v>5.2</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>97</v>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="B94" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C94" s="2">
         <v>5.2</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>98</v>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="B95" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C95" s="2">
         <v>7.1</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>99</v>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="B96" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C96" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>100</v>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="B97" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C97" s="2">
         <v>6.9</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>101</v>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="B98" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C98" s="2">
         <v>6.9</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>102</v>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="B99" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C99" s="2">
         <v>5.7</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>103</v>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="B100" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C100" s="2">
         <v>4.7</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>104</v>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="B101" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C101" s="2">
         <v>5.6</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>105</v>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="B102" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C102" s="2">
-        <v>8.3</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>106</v>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="B103" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C103" s="2">
         <v>9.9</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>107</v>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="B104" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C104" s="2">
         <v>12.5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>108</v>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="B105" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C105" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>109</v>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="B106" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C106" s="2">
         <v>14.4</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>110</v>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="B107" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C107" s="2">
-        <v>16.4</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>111</v>
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="B108" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C108" s="2">
         <v>16.7</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>112</v>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="B109" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C109" s="2">
         <v>17.7</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>113</v>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="4" t="s">
+        <v>103</v>
       </c>
       <c r="B110" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C110" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>114</v>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="B111" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C111" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>115</v>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="B112" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C112" s="2">
         <v>14.3</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>116</v>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="B113" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C113" s="2">
         <v>13.1</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>117</v>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="B114" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C114" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>118</v>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="B115" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C115" s="2">
         <v>13.8</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>119</v>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="B116" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C116" s="2">
         <v>14.3</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>120</v>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="B117" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C117" s="2">
         <v>13.3</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>121</v>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="B118" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C118" s="2">
         <v>13.6</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>122</v>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="B119" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C119" s="2">
         <v>13.3</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>123</v>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="B120" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C120" s="2">
         <v>9.4</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>124</v>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="B121" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C121" s="2">
-        <v>8.7</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>125</v>
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="B122" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C122" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>126</v>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="B123" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C123" s="2">
         <v>7.8</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
-        <v>127</v>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="B124" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C124" s="2">
         <v>7.6</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
-        <v>128</v>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="B125" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C125" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
-        <v>129</v>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="B126" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C126" s="2">
-        <v>8.8</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>130</v>
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="B127" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C127" s="2">
         <v>9.5</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
-        <v>131</v>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="B128" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C128" s="2">
-        <v>10.2</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
-        <v>132</v>
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="B129" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C129" s="2">
         <v>10.4</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
-        <v>133</v>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="B130" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C130" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
-        <v>134</v>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="B131" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C131" s="2">
         <v>9.9</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
-        <v>135</v>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="B132" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C132" s="2">
-        <v>9.2</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
-        <v>136</v>
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="B133" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C133" s="2">
         <v>9.4</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
-        <v>137</v>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="B134" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C134" s="2">
         <v>8.4</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
-        <v>138</v>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" s="4" t="s">
+        <v>128</v>
       </c>
       <c r="B135" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C135" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
-        <v>139</v>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="B136" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C136" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
-        <v>140</v>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="B137" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C137" s="2">
         <v>10.8</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
-        <v>141</v>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="B138" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C138" s="2">
         <v>10.9</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
-        <v>142</v>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="B139" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C139" s="2">
         <v>12.4</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
-        <v>143</v>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="B140" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C140" s="2">
         <v>11.3</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
-        <v>144</v>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="B141" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C141" s="2">
         <v>11.4</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
-        <v>145</v>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" s="4" t="s">
+        <v>135</v>
       </c>
       <c r="B142" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C142" s="2">
         <v>11.1</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="1" t="s">
-        <v>146</v>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" s="4" t="s">
+        <v>136</v>
       </c>
       <c r="B143" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C143" s="2">
-        <v>9.2</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
-        <v>147</v>
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="B144" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C144" s="2">
         <v>8.6</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
-        <v>148</v>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145" s="4" t="s">
+        <v>138</v>
       </c>
       <c r="B145" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C145" s="2">
         <v>5.8</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
-        <v>149</v>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="B146" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C146" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="1" t="s">
-        <v>150</v>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="B147" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C147" s="2">
         <v>3.7</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
-        <v>151</v>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="B148" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C148" s="2">
         <v>2.5</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
-        <v>152</v>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="B149" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C149" s="2">
-        <v>4.4</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
-        <v>153</v>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150" s="4" t="s">
+        <v>143</v>
       </c>
       <c r="B150" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C150" s="2">
         <v>6.6</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" s="1" t="s">
-        <v>154</v>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A151" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="B151" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C151" s="2">
         <v>7.6</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="1" t="s">
-        <v>155</v>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A152" s="4" t="s">
+        <v>145</v>
       </c>
       <c r="B152" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C152" s="2">
-        <v>8.3</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="1" t="s">
-        <v>156</v>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A153" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="B153" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C153" s="2">
-        <v>9.2</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
-        <v>157</v>
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A154" s="4" t="s">
+        <v>147</v>
       </c>
       <c r="B154" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C154" s="2">
         <v>8.5</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="1" t="s">
-        <v>158</v>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A155" s="4" t="s">
+        <v>148</v>
       </c>
       <c r="B155" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C155" s="2">
-        <v>8.8</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" s="1" t="s">
-        <v>159</v>
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A156" s="4" t="s">
+        <v>149</v>
       </c>
       <c r="B156" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C156" s="2">
         <v>9.6</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" s="1" t="s">
-        <v>160</v>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A157" s="4" t="s">
+        <v>150</v>
       </c>
       <c r="B157" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C157" s="2">
         <v>9.4</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
-        <v>161</v>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A158" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="B158" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C158" s="2">
-        <v>9.3</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" s="1" t="s">
-        <v>162</v>
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A159" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="B159" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C159" s="2">
-        <v>8.3</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160" s="1" t="s">
-        <v>163</v>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A160" s="4" t="s">
+        <v>153</v>
       </c>
       <c r="B160" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C160" s="2">
         <v>7.2</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="1" t="s">
-        <v>164</v>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A161" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="B161" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C161" s="2">
         <v>6.8</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
-        <v>165</v>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="B162" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C162" s="2">
         <v>7.2</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="1" t="s">
-        <v>166</v>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A163" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="B163" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C163" s="2">
         <v>7.3</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="1" t="s">
-        <v>167</v>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="B164" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C164" s="2">
         <v>7.6</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165" s="1" t="s">
-        <v>168</v>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A165" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="B165" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C165" s="2">
         <v>6.8</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" s="1" t="s">
-        <v>169</v>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A166" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="B166" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C166" s="2">
         <v>7.5</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="1" t="s">
-        <v>170</v>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A167" s="4" t="s">
+        <v>160</v>
       </c>
       <c r="B167" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C167" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="1" t="s">
-        <v>171</v>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A168" s="4" t="s">
+        <v>161</v>
       </c>
       <c r="B168" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C168" s="2">
         <v>7.8</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" s="1" t="s">
-        <v>172</v>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A169" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="B169" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C169" s="2">
-        <v>8.7</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" s="1" t="s">
-        <v>173</v>
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A170" s="4" t="s">
+        <v>163</v>
       </c>
       <c r="B170" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C170" s="2">
         <v>7.7</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" s="1" t="s">
-        <v>174</v>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A171" s="4" t="s">
+        <v>164</v>
       </c>
       <c r="B171" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C171" s="2">
         <v>6.1</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="1" t="s">
-        <v>175</v>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A172" s="4" t="s">
+        <v>165</v>
       </c>
       <c r="B172" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C172" s="2">
         <v>6.9</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" s="1" t="s">
-        <v>176</v>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A173" s="4" t="s">
+        <v>166</v>
       </c>
       <c r="B173" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C173" s="2">
         <v>4.8</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="1" t="s">
-        <v>177</v>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="B174" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C174" s="2">
         <v>3.3</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="1" t="s">
-        <v>178</v>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A175" s="4" t="s">
+        <v>168</v>
       </c>
       <c r="B175" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C175" s="2">
         <v>3.1</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" s="1" t="s">
-        <v>179</v>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A176" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="B176" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C176" s="2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" s="1" t="s">
-        <v>180</v>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A177" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="B177" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C177" s="2">
         <v>1.7</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" s="1" t="s">
-        <v>181</v>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A178" s="4" t="s">
+        <v>171</v>
       </c>
       <c r="B178" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C178" s="2">
         <v>1.2</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" s="1" t="s">
-        <v>182</v>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A179" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="B179" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C179" s="2">
         <v>0.8</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" s="1" t="s">
-        <v>183</v>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A180" s="4" t="s">
+        <v>173</v>
       </c>
       <c r="B180" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C180" s="2">
         <v>0.3</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" s="1" t="s">
-        <v>184</v>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A181" s="4" t="s">
+        <v>174</v>
       </c>
       <c r="B181" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C181" s="2">
         <v>1.2</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" s="1" t="s">
-        <v>185</v>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A182" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="B182" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C182" s="2">
         <v>1.8</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" s="1" t="s">
-        <v>186</v>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A183" s="4" t="s">
+        <v>176</v>
       </c>
       <c r="B183" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C183" s="2">
-        <v>2.2</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" s="1" t="s">
-        <v>188</v>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A184" s="4" t="s">
+        <v>178</v>
       </c>
       <c r="B184" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C184" s="2">
         <v>1.8</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" s="1" t="s">
-        <v>189</v>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A185" s="4" t="s">
+        <v>179</v>
       </c>
       <c r="B185" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C185" s="2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A186" s="1" t="s">
-        <v>190</v>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A186" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="B186" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C186" s="2">
         <v>1.8</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A187" s="1" t="s">
-        <v>191</v>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A187" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="B187" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C187" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" s="1" t="s">
-        <v>192</v>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A188" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="B188" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C188" s="2">
         <v>2.6</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189" s="1" t="s">
-        <v>193</v>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A189" s="4" t="s">
+        <v>183</v>
       </c>
       <c r="B189" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C189" s="2">
         <v>3.7</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A190" s="1" t="s">
-        <v>194</v>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A190" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="B190" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C190" s="2">
         <v>4.5</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A191" s="1" t="s">
-        <v>195</v>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A191" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="B191" t="s">
+        <v>177</v>
+      </c>
+      <c r="C191" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A192" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B192" t="s">
+        <v>177</v>
+      </c>
+      <c r="C192" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A193" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C191" s="2">
-        <v>5.1</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B192" t="s">
-        <v>187</v>
-      </c>
-      <c r="C192" s="2">
-        <v>5.1</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="B193" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C193" s="2">
         <v>3.8</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" s="1" t="s">
-        <v>198</v>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A194" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="B194" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C194" s="2">
         <v>3.1</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" s="1" t="s">
-        <v>199</v>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A195" s="4" t="s">
+        <v>189</v>
       </c>
       <c r="B195" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C195" s="2">
         <v>2.1</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196" s="1" t="s">
-        <v>200</v>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A196" s="4" t="s">
+        <v>190</v>
       </c>
       <c r="B196" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C196" s="2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" s="1" t="s">
-        <v>201</v>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A197" s="4" t="s">
+        <v>191</v>
       </c>
       <c r="B197" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C197" s="2">
         <v>1.4</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" s="1" t="s">
-        <v>202</v>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A198" s="4" t="s">
+        <v>192</v>
       </c>
       <c r="B198" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C198" s="2">
         <v>0.3</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" s="1" t="s">
-        <v>203</v>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A199" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="B199" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C199" s="2">
         <v>-0.4</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200" s="1" t="s">
-        <v>204</v>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A200" s="4" t="s">
+        <v>194</v>
       </c>
       <c r="B200" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C200" s="2">
         <v>-0.3</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" s="1" t="s">
-        <v>205</v>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A201" s="4" t="s">
+        <v>195</v>
       </c>
       <c r="B201" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C201" s="2">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" s="1" t="s">
-        <v>206</v>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A202" s="4" t="s">
+        <v>196</v>
       </c>
       <c r="B202" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C202" s="2">
         <v>0.7</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A203" s="1" t="s">
-        <v>207</v>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A203" s="4" t="s">
+        <v>197</v>
       </c>
       <c r="B203" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C203" s="2">
         <v>1.4</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" s="1" t="s">
-        <v>208</v>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A204" s="4" t="s">
+        <v>198</v>
       </c>
       <c r="B204" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C204" s="2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205" s="1" t="s">
-        <v>209</v>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A205" s="4" t="s">
+        <v>199</v>
       </c>
       <c r="B205" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C205" s="2">
         <v>1.2</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A206" s="1" t="s">
-        <v>210</v>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A206" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="B206" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C206" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" s="1" t="s">
-        <v>211</v>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A207" s="4" t="s">
+        <v>201</v>
       </c>
       <c r="B207" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C207" s="2">
         <v>1.8</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" s="1" t="s">
-        <v>212</v>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A208" s="4" t="s">
+        <v>202</v>
       </c>
       <c r="B208" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C208" s="2">
         <v>1.9</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A209" s="1" t="s">
-        <v>213</v>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A209" s="4" t="s">
+        <v>203</v>
       </c>
       <c r="B209" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C209" s="2">
         <v>2.8</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210" s="1" t="s">
-        <v>214</v>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A210" s="4" t="s">
+        <v>204</v>
       </c>
       <c r="B210" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C210" s="2">
         <v>3.1</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" s="1" t="s">
-        <v>215</v>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A211" s="4" t="s">
+        <v>205</v>
       </c>
       <c r="B211" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C211" s="2">
         <v>6.1</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212" s="1" t="s">
-        <v>216</v>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A212" s="4" t="s">
+        <v>206</v>
       </c>
       <c r="B212" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C212" s="2">
         <v>5.8</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A213" s="1" t="s">
-        <v>217</v>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A213" s="4" t="s">
+        <v>207</v>
       </c>
       <c r="B213" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C213" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A214" s="1" t="s">
-        <v>218</v>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A214" s="4" t="s">
+        <v>208</v>
       </c>
       <c r="B214" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C214" s="2">
         <v>6.1</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215" s="1" t="s">
-        <v>219</v>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A215" s="4" t="s">
+        <v>209</v>
       </c>
       <c r="B215" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C215" s="2">
         <v>2.5</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A216" s="1" t="s">
-        <v>220</v>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A216" s="4" t="s">
+        <v>210</v>
       </c>
       <c r="B216" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C216" s="2">
         <v>3.1</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A217" s="1" t="s">
-        <v>221</v>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A217" s="4" t="s">
+        <v>211</v>
       </c>
       <c r="B217" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C217" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A218" s="1" t="s">
-        <v>222</v>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A218" s="4" t="s">
+        <v>212</v>
       </c>
       <c r="B218" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C218" s="2">
         <v>2.8</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A219" s="1" t="s">
-        <v>223</v>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A219" s="4" t="s">
+        <v>213</v>
       </c>
       <c r="B219" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C219" s="2">
         <v>3.2</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A220" s="1" t="s">
-        <v>224</v>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A220" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="B220" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C220" s="2">
         <v>2.9</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A221" s="1" t="s">
-        <v>225</v>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A221" s="4" t="s">
+        <v>215</v>
       </c>
       <c r="B221" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C221" s="2">
         <v>3.3</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A222" s="1" t="s">
-        <v>226</v>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A222" s="4" t="s">
+        <v>216</v>
       </c>
       <c r="B222" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C222" s="2">
         <v>2.6</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A223" s="1" t="s">
-        <v>227</v>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A223" s="4" t="s">
+        <v>217</v>
       </c>
       <c r="B223" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C223" s="2">
         <v>2.6</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A224" s="1" t="s">
-        <v>228</v>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A224" s="4" t="s">
+        <v>218</v>
       </c>
       <c r="B224" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C224" s="2">
         <v>2.4</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A225" s="1" t="s">
-        <v>229</v>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A225" s="4" t="s">
+        <v>219</v>
       </c>
       <c r="B225" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C225" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A226" s="1" t="s">
-        <v>230</v>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A226" s="4" t="s">
+        <v>220</v>
       </c>
       <c r="B226" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C226" s="2">
         <v>2.5</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A227" s="1" t="s">
-        <v>231</v>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A227" s="4" t="s">
+        <v>221</v>
       </c>
       <c r="B227" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C227" s="2">
-        <v>2.3</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A228" s="1" t="s">
-        <v>232</v>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A228" s="4" t="s">
+        <v>222</v>
       </c>
       <c r="B228" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C228" s="2">
         <v>2.5</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A229" s="1" t="s">
-        <v>233</v>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A229" s="4" t="s">
+        <v>223</v>
       </c>
       <c r="B229" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C229" s="2">
         <v>2.4</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A230" s="1" t="s">
-        <v>234</v>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A230" s="4" t="s">
+        <v>224</v>
       </c>
       <c r="B230" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C230" s="2">
         <v>2.5</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A231" s="1" t="s">
-        <v>235</v>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A231" s="4" t="s">
+        <v>225</v>
       </c>
       <c r="B231" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C231" s="2">
         <v>3.1</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A232" s="1" t="s">
-        <v>236</v>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A232" s="4" t="s">
+        <v>226</v>
       </c>
       <c r="B232" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C232" s="2">
         <v>2.8</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A233" s="1" t="s">
-        <v>237</v>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A233" s="4" t="s">
+        <v>227</v>
       </c>
       <c r="B233" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C233" s="2">
         <v>2.9</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A234" s="1" t="s">
-        <v>238</v>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A234" s="4" t="s">
+        <v>228</v>
       </c>
       <c r="B234" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C234" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A235" s="1" t="s">
-        <v>239</v>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A235" s="4" t="s">
+        <v>229</v>
       </c>
       <c r="B235" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C235" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A236" s="1" t="s">
-        <v>240</v>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A236" s="4" t="s">
+        <v>230</v>
       </c>
       <c r="B236" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C236" s="2">
         <v>3.3</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A237" s="1" t="s">
-        <v>241</v>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A237" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="B237" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C237" s="2">
         <v>2.5</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A238" s="1" t="s">
-        <v>242</v>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A238" s="4" t="s">
+        <v>232</v>
       </c>
       <c r="B238" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C238" s="2">
         <v>2.1</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A239" s="1" t="s">
-        <v>243</v>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A239" s="4" t="s">
+        <v>233</v>
       </c>
       <c r="B239" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C239" s="2">
         <v>1.8</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A240" s="1" t="s">
-        <v>244</v>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A240" s="4" t="s">
+        <v>234</v>
       </c>
       <c r="B240" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C240" s="2">
         <v>2.9</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A241" s="1" t="s">
-        <v>245</v>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A241" s="4" t="s">
+        <v>235</v>
       </c>
       <c r="B241" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C241" s="2">
         <v>4.3</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A242" s="1" t="s">
-        <v>246</v>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A242" s="4" t="s">
+        <v>236</v>
       </c>
       <c r="B242" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C242" s="2">
-        <v>4.4</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A243" s="1" t="s">
-        <v>247</v>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A243" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="B243" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C243" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A244" s="1" t="s">
-        <v>248</v>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A244" s="4" t="s">
+        <v>238</v>
       </c>
       <c r="B244" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C244" s="2">
         <v>3.7</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A245" s="1" t="s">
-        <v>249</v>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A245" s="4" t="s">
+        <v>239</v>
       </c>
       <c r="B245" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C245" s="2">
         <v>2.4</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A246" s="1" t="s">
-        <v>250</v>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A246" s="4" t="s">
+        <v>240</v>
       </c>
       <c r="B246" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C246" s="2">
         <v>1.4</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A247" s="1" t="s">
-        <v>251</v>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A247" s="4" t="s">
+        <v>241</v>
       </c>
       <c r="B247" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C247" s="2">
         <v>1.2</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A248" s="1" t="s">
-        <v>252</v>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A248" s="4" t="s">
+        <v>242</v>
       </c>
       <c r="B248" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C248" s="2">
         <v>2.1</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A249" s="1" t="s">
-        <v>253</v>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A249" s="4" t="s">
+        <v>243</v>
       </c>
       <c r="B249" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C249" s="2">
         <v>2.9</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A250" s="1" t="s">
-        <v>254</v>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A250" s="4" t="s">
+        <v>244</v>
       </c>
       <c r="B250" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C250" s="2">
         <v>3.1</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A251" s="1" t="s">
-        <v>255</v>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A251" s="4" t="s">
+        <v>245</v>
       </c>
       <c r="B251" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C251" s="2">
         <v>2.9</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A252" s="1" t="s">
-        <v>256</v>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A252" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="B252" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C252" s="2">
         <v>2.8</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A253" s="1" t="s">
-        <v>257</v>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A253" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="B253" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C253" s="2">
         <v>3.3</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A254" s="1" t="s">
-        <v>258</v>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A254" s="4" t="s">
+        <v>248</v>
       </c>
       <c r="B254" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C254" s="2">
         <v>3.5</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A255" s="1" t="s">
-        <v>259</v>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A255" s="4" t="s">
+        <v>249</v>
       </c>
       <c r="B255" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C255" s="2">
         <v>3.4</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A256" s="1" t="s">
-        <v>260</v>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A256" s="4" t="s">
+        <v>250</v>
       </c>
       <c r="B256" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C256" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A257" s="1" t="s">
-        <v>261</v>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A257" s="4" t="s">
+        <v>251</v>
       </c>
       <c r="B257" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C257" s="2">
         <v>1.6</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A258" s="1" t="s">
-        <v>262</v>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A258" s="4" t="s">
+        <v>252</v>
       </c>
       <c r="B258" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C258" s="2">
         <v>1.2</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A259" s="1" t="s">
-        <v>263</v>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A259" s="4" t="s">
+        <v>253</v>
       </c>
       <c r="B259" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C259" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A260" s="1" t="s">
-        <v>264</v>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A260" s="4" t="s">
+        <v>254</v>
       </c>
       <c r="B260" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C260" s="2">
-        <v>2.2</v>
-      </c>
-    </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A261" s="1" t="s">
-        <v>265</v>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A261" s="4" t="s">
+        <v>255</v>
       </c>
       <c r="B261" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C261" s="2">
         <v>2.5</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A262" s="1" t="s">
-        <v>266</v>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A262" s="4" t="s">
+        <v>256</v>
       </c>
       <c r="B262" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C262" s="2">
         <v>2.4</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A263" s="1" t="s">
-        <v>267</v>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A263" s="4" t="s">
+        <v>257</v>
       </c>
       <c r="B263" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C263" s="2">
-        <v>2.2</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A264" s="1" t="s">
-        <v>268</v>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A264" s="4" t="s">
+        <v>258</v>
       </c>
       <c r="B264" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C264" s="2">
         <v>2.7</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A265" s="1" t="s">
-        <v>269</v>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A265" s="4" t="s">
+        <v>259</v>
       </c>
       <c r="B265" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C265" s="2">
         <v>2.9</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A266" s="1" t="s">
-        <v>270</v>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A266" s="4" t="s">
+        <v>260</v>
       </c>
       <c r="B266" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C266" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A267" s="1" t="s">
-        <v>271</v>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A267" s="4" t="s">
+        <v>261</v>
       </c>
       <c r="B267" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C267" s="2">
-        <v>2.3</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A268" s="1" t="s">
-        <v>272</v>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A268" s="4" t="s">
+        <v>262</v>
       </c>
       <c r="B268" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C268" s="2">
         <v>1.7</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A269" s="1" t="s">
-        <v>273</v>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A269" s="4" t="s">
+        <v>263</v>
       </c>
       <c r="B269" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C269" s="2">
         <v>1.3</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A270" s="1" t="s">
-        <v>274</v>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A270" s="4" t="s">
+        <v>264</v>
       </c>
       <c r="B270" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C270" s="2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A271" s="1" t="s">
-        <v>275</v>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A271" s="4" t="s">
+        <v>265</v>
       </c>
       <c r="B271" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C271" s="2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A272" s="1" t="s">
-        <v>276</v>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A272" s="4" t="s">
+        <v>266</v>
       </c>
       <c r="B272" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C272" s="2">
         <v>1.7</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A273" s="1" t="s">
-        <v>277</v>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A273" s="4" t="s">
+        <v>267</v>
       </c>
       <c r="B273" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C273" s="2">
         <v>1.3</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A274" s="1" t="s">
-        <v>278</v>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A274" s="4" t="s">
+        <v>268</v>
       </c>
       <c r="B274" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C274" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A275" s="1" t="s">
-        <v>279</v>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A275" s="4" t="s">
+        <v>269</v>
       </c>
       <c r="B275" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C275" s="2">
         <v>1.3</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A276" s="1" t="s">
-        <v>280</v>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A276" s="4" t="s">
+        <v>270</v>
       </c>
       <c r="B276" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C276" s="2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A277" s="1" t="s">
-        <v>281</v>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A277" s="4" t="s">
+        <v>271</v>
       </c>
       <c r="B277" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C277" s="2">
         <v>2.1</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A278" s="1" t="s">
-        <v>282</v>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A278" s="4" t="s">
+        <v>272</v>
       </c>
       <c r="B278" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C278" s="2">
         <v>1.9</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A279" s="1" t="s">
-        <v>283</v>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A279" s="4" t="s">
+        <v>273</v>
       </c>
       <c r="B279" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C279" s="2">
         <v>1.8</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A280" s="1" t="s">
-        <v>284</v>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A280" s="4" t="s">
+        <v>274</v>
       </c>
       <c r="B280" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C280" s="2">
         <v>1.9</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A281" s="1" t="s">
-        <v>285</v>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A281" s="4" t="s">
+        <v>275</v>
       </c>
       <c r="B281" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C281" s="2">
         <v>1.9</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A282" s="1" t="s">
-        <v>286</v>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A282" s="4" t="s">
+        <v>276</v>
       </c>
       <c r="B282" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C282" s="2">
         <v>2.1</v>
       </c>
     </row>
-    <row r="284" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A284" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A285" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A286" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A287" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A288" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A289" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A290" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A291" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A292" s="3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A293" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A294" s="3" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="285" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A285" s="3" t="s">
+    <row r="295" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A295" s="3" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="286" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A286" s="3" t="s">
+    <row r="296" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A296" s="3" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="287" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A287" s="3" t="s">
+    <row r="297" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A297" s="3" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="288" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A288" s="3" t="s">
+    <row r="298" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A298" s="3" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="289" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A289" s="3" t="s">
+    <row r="299" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A299" s="3" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="290" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A290" s="3" t="s">
+    <row r="300" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A300" s="3" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="291" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A291" s="3" t="s">
+    <row r="301" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A301" s="3" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="292" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A292" s="3" t="s">
+    <row r="302" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A302" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="293" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A293" s="3" t="s">
+    <row r="303" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A303" s="3" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="294" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A294" s="3" t="s">
+    <row r="304" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A304" s="3" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="295" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A295" s="3" t="s">
+    <row r="305" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A305" s="3" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="296" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A296" s="3" t="s">
+    <row r="306" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A306" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="297" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A297" s="3" t="s">
+    <row r="307" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A307" s="3" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="298" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A298" s="3" t="s">
+    <row r="309" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A309" s="3" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="299" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A299" s="3" t="s">
+    <row r="310" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A310" s="3" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="300" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A300" s="3" t="s">
+    <row r="311" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A311" s="3" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="301" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A301" s="3" t="s">
+    <row r="312" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A312" s="3" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="302" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A302" s="3" t="s">
+    <row r="313" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A313" s="3" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="303" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A303" s="3" t="s">
+    <row r="314" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A314" s="3" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="304" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A304" s="3" t="s">
+    <row r="315" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A315" s="3" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="305" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A305" s="3" t="s">
+    <row r="316" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A316" s="3" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="306" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A306" s="3" t="s">
+    <row r="317" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A317" s="3" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="307" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A307" s="3" t="s">
+    <row r="318" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A318" s="3" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="309" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A309" s="3" t="s">
+    <row r="319" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A319" s="3" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="310" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A310" s="3" t="s">
+    <row r="320" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A320" s="3" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="311" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A311" s="3" t="s">
+    <row r="321" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A321" s="3" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="312" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A312" s="3" t="s">
+    <row r="322" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A322" s="3" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="313" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A313" s="3" t="s">
+    <row r="323" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A323" s="3" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="314" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A314" s="3" t="s">
+    <row r="324" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A324" s="3" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="315" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A315" s="3" t="s">
+    <row r="325" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A325" s="3" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="316" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A316" s="3" t="s">
+    <row r="326" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A326" s="3" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="317" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A317" s="3" t="s">
+    <row r="327" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A327" s="3" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="318" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A318" s="3" t="s">
+    <row r="328" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A328" s="3" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="319" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A319" s="3" t="s">
+    <row r="329" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A329" s="3" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="320" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A320" s="3" t="s">
+    <row r="330" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A330" s="3" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="321" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A321" s="3" t="s">
+    <row r="331" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A331" s="3" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="322" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A322" s="3" t="s">
+    <row r="332" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A332" s="3" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="323" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A323" s="3" t="s">
+    <row r="334" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A334" s="3" t="s">
         <v>325</v>
-      </c>
-    </row>
-    <row r="324" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A324" s="3" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="325" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A325" s="3" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="326" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A326" s="3" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="327" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A327" s="3" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="328" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A328" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="329" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A329" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="330" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A330" s="3" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="331" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A331" s="3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="332" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A332" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="334" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A334" s="3" t="s">
-        <v>335</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <ignoredErrors>
+    <ignoredError sqref="A13:A282" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>